<commit_message>
Updated readme and velocity graph and also added link to site in each file
</commit_message>
<xml_diff>
--- a/Required Files/veloicity graph.xlsx
+++ b/Required Files/veloicity graph.xlsx
@@ -5,17 +5,17 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kkanishkan/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kkanishkan/Desktop/iteration2and2/src/Required Files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1A6089A6-4271-3B46-9309-39EBD1EC8FB6}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E00B1E0-4B13-AB40-91A7-A2F4DE8204F4}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2780" yWindow="1560" windowWidth="28040" windowHeight="17440" xr2:uid="{0B4F6A34-BDDA-E849-A5C5-AC6837F2611F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -251,22 +251,22 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="4">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>1</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>1</c:v>
@@ -353,28 +353,28 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>3</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>5</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>12</c:v>
+                  <c:v>7.5</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>12</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1572,10 +1572,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A0CD6D64-52FE-5140-B147-F75CB67D7A4C}">
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1608,7 +1608,7 @@
         <v>1</v>
       </c>
       <c r="C3">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
@@ -1616,10 +1616,10 @@
         <v>43560</v>
       </c>
       <c r="B4">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C4">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
@@ -1630,7 +1630,7 @@
         <v>3</v>
       </c>
       <c r="C5">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
@@ -1638,10 +1638,10 @@
         <v>43562</v>
       </c>
       <c r="B6">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C6">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
@@ -1649,7 +1649,7 @@
         <v>43563</v>
       </c>
       <c r="B7">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C7">
         <v>1</v>
@@ -1660,10 +1660,10 @@
         <v>43564</v>
       </c>
       <c r="B8">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C8">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
@@ -1671,10 +1671,10 @@
         <v>43565</v>
       </c>
       <c r="B9">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C9">
-        <v>12</v>
+        <v>7.5</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
@@ -1685,7 +1685,17 @@
         <v>1</v>
       </c>
       <c r="C10">
-        <v>12</v>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B11">
+        <f>SUM(B3:B10)</f>
+        <v>16</v>
+      </c>
+      <c r="C11">
+        <f>SUM(C3:C10)</f>
+        <v>21.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>